<commit_message>
Completed Balance Sheet development
Completed Balance Sheet development
</commit_message>
<xml_diff>
--- a/DataMappings.xlsx
+++ b/DataMappings.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="217">
   <si>
     <t>Field Name</t>
   </si>
@@ -603,6 +603,9 @@
   </si>
   <si>
     <t>PRE</t>
+  </si>
+  <si>
+    <t>DIM_PREPERATION_OF_STATEMENTS</t>
   </si>
   <si>
     <t>report</t>
@@ -1319,7 +1322,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1333,6 +1336,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
@@ -2973,7 +2979,7 @@
       <c r="G2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2999,7 +3005,7 @@
       <c r="G3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3023,7 +3029,7 @@
         <v>13</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="6" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3047,7 +3053,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="6" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3071,7 +3077,7 @@
         <v>29</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="6" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3095,7 +3101,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="6" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3119,7 +3125,7 @@
         <v>29</v>
       </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="6" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3143,7 +3149,7 @@
         <v>29</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="6" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3165,7 +3171,7 @@
         <v>29</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="6" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3180,8 +3186,8 @@
   <sheetPr/>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="51.7777777777778" defaultRowHeight="14.4"/>
@@ -3251,7 +3257,7 @@
       <c r="H2" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3280,7 +3286,7 @@
       <c r="H3" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="6" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3309,7 +3315,7 @@
       <c r="H4" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="6" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3338,7 +3344,7 @@
       <c r="H5" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="6" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3367,7 +3373,7 @@
       <c r="H6" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="6" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3396,7 +3402,7 @@
       <c r="H7" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="6" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3425,7 +3431,7 @@
       <c r="H8" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="6" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3454,7 +3460,7 @@
       <c r="H9" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="6" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3481,7 +3487,7 @@
       <c r="H10" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="6" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3508,7 +3514,7 @@
       <c r="H11" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="6" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3521,13 +3527,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="68.2222222222222" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="68.2222222222222" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.1111111111111" customWidth="1"/>
     <col min="2" max="2" width="67.1111111111111" customWidth="1"/>
@@ -3540,7 +3546,7 @@
     <col min="9" max="16384" width="68.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3565,8 +3571,11 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" ht="28.8" spans="1:8">
+      <c r="I1" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" ht="28.8" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -3591,13 +3600,16 @@
       <c r="H2" s="3" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="3" ht="43.2" spans="1:8">
+      <c r="I2" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" ht="43.2" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>19</v>
@@ -3615,15 +3627,18 @@
         <v>189</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="4" ht="43.2" spans="1:8">
+        <v>193</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" ht="43.2" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>19</v>
@@ -3641,18 +3656,21 @@
         <v>189</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="5" ht="43.2" spans="1:8">
+        <v>196</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" ht="43.2" spans="1:9">
       <c r="A5" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D5" s="3">
         <v>2</v>
@@ -3665,15 +3683,18 @@
         <v>189</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="6" ht="43.2" spans="1:8">
+        <v>200</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" ht="43.2" spans="1:9">
       <c r="A6" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>145</v>
@@ -3689,15 +3710,18 @@
         <v>189</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="7" ht="28.8" spans="1:8">
+        <v>203</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" ht="28.8" spans="1:9">
       <c r="A7" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>25</v>
@@ -3713,15 +3737,18 @@
         <v>189</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="8" ht="28.8" spans="1:8">
+        <v>206</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" ht="28.8" spans="1:9">
       <c r="A8" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>25</v>
@@ -3739,15 +3766,18 @@
         <v>189</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="9" ht="28.8" spans="1:8">
+        <v>208</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" ht="28.8" spans="1:9">
       <c r="A9" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>25</v>
@@ -3765,15 +3795,18 @@
         <v>189</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="10" ht="28.8" spans="1:8">
+        <v>210</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" ht="28.8" spans="1:9">
       <c r="A10" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>25</v>
@@ -3789,15 +3822,18 @@
         <v>189</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="11" ht="28.8" spans="1:8">
+        <v>213</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" ht="28.8" spans="1:9">
       <c r="A11" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>145</v>
@@ -3813,7 +3849,10 @@
         <v>189</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>